<commit_message>
Finished extra kpis, charts, expr builder for costs drillthrough chart, connecting filters, data browsers.
Note that timeseries filter is currently broken by timeline faceting on costs charts after several uses, appears to be an open issue so will need alternate coding around it.
</commit_message>
<xml_diff>
--- a/app/data/comparison sets/parameters.xlsx
+++ b/app/data/comparison sets/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\OneDrive\Desktop\Ecodata\Repos\mars_rhino\app\data\comparison sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89E376B-FC97-440E-8EF1-FA7E310CCCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E907C4A6-ECBF-4D6E-81C2-CEB058EF5A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
   <si>
     <t>parameter</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>White Teak_Calendar</t>
+  </si>
+  <si>
+    <t>monthly_income_threshold_rp</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,6 +581,14 @@
       </c>
       <c r="B6">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1">
+        <v>25000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added plot aggregation to year and parameter set exporting
</commit_message>
<xml_diff>
--- a/app/data/comparison sets/parameters.xlsx
+++ b/app/data/comparison sets/parameters.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\OneDrive\Desktop\Ecodata\Repos\mars_rhino\app\data\comparison sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E907C4A6-ECBF-4D6E-81C2-CEB058EF5A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B37110-1CA4-4AB8-9B16-B6653210B181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="64305" yWindow="3075" windowWidth="23265" windowHeight="12795" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation_control" sheetId="1" r:id="rId1"/>
     <sheet name="crop_global_parameters" sheetId="4" r:id="rId2"/>
     <sheet name="farm_layout" sheetId="2" r:id="rId3"/>
     <sheet name="farm_layout full" sheetId="6" r:id="rId4"/>
-    <sheet name="crop sheet lookup" sheetId="5" r:id="rId5"/>
+    <sheet name="crop_sheet_lookup" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -526,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1363,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C074F89E-2346-4E9E-B992-B11A467BD05A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>